<commit_message>
Corrected Calibration and Ingest Sheets for Coastal Gliders
Changed FLORT cal values for angular resolution  to 1.076, changed
Scattering Angle to 124.  Added ADCP line to ingest files for Endurance
recovered gliders.  INcluded changes to templates.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL###/Omaha_Cal_Info_CE05MOAS-GL###_0000#.xlsx
+++ b/CE05MOAS-GL###/Omaha_Cal_Info_CE05MOAS-GL###_0000#.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12405" tabRatio="377" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12405" tabRatio="377" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -2094,7 +2094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -2249,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,7 +2344,7 @@
         <v>48</v>
       </c>
       <c r="F4" s="39">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>47</v>
@@ -2400,7 +2400,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="39">
-        <v>1.08</v>
+        <v>1.0760000000000001</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>47</v>

</xml_diff>